<commit_message>
Formulario de inventario terminado
</commit_message>
<xml_diff>
--- a/Datos/productos.xlsx
+++ b/Datos/productos.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R390ae22cbb994191"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R1e6714e3bc774f1f"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <x:si>
     <x:t>Codigo</x:t>
   </x:si>
@@ -41,13 +41,7 @@
     <x:t>perfume</x:t>
   </x:si>
   <x:si>
-    <x:t>..\..\Imagenes\222-perfume.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>cerveza</x:t>
-  </x:si>
-  <x:si>
-    <x:t>..\..\Imagenes\3-dsfsd.jpg</x:t>
+    <x:t>..\..\Imagenes\2324567-perfume.jpg</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -387,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F4"/>
+  <x:dimension ref="A1:F3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -415,7 +409,7 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>123456</x:v>
+        <x:v>1234456</x:v>
       </x:c>
       <x:c r="B2" t="s">
         <x:v>6</x:v>
@@ -427,7 +421,7 @@
         <x:v>321</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>123</x:v>
+        <x:v>12.32</x:v>
       </x:c>
       <x:c r="F2">
         <x:v>231</x:v>
@@ -435,7 +429,7 @@
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>234567</x:v>
+        <x:v>2324567</x:v>
       </x:c>
       <x:c r="B3" t="s">
         <x:v>8</x:v>
@@ -451,26 +445,6 @@
       </x:c>
       <x:c r="F3">
         <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4">
-      <x:c r="A4">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B4" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C4" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D4">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E4">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="F4">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Modificacion en formulario factura 90%
</commit_message>
<xml_diff>
--- a/Datos/productos.xlsx
+++ b/Datos/productos.xlsx
@@ -1,99 +1,136 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="SpreadsheetLight"/>
-  <x:bookViews>
-    <x:workbookView/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R1e6714e3bc774f1f"/>
-  </x:sheets>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UDB\CICLO III\Programación con Estructuras de Datos\Proyecto\PROYECTO\Datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4217796-0A3B-49B1-9053-105AA3A2BA51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <x:si>
-    <x:t>Codigo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Descripcion</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ruta_imagen</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Precio_compra</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Precio_venta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Existencia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>jabon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>..\..\Imagenes\2332-jabon.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>perfume</x:t>
-  </x:si>
-  <x:si>
-    <x:t>..\..\Imagenes\2324567-perfume.jpg</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Ruta_imagen</t>
+  </si>
+  <si>
+    <t>Precio_compra</t>
+  </si>
+  <si>
+    <t>Precio_venta</t>
+  </si>
+  <si>
+    <t>Existencia</t>
+  </si>
+  <si>
+    <t>..\..\Imagenes\2332-jabon.jpg</t>
+  </si>
+  <si>
+    <t>..\..\Imagenes\2324567-perfume.jpg</t>
+  </si>
+  <si>
+    <t>llanta</t>
+  </si>
+  <si>
+    <t>..\..\Imagenes\4534534-llanta.jpg</t>
+  </si>
+  <si>
+    <t>pintura</t>
+  </si>
+  <si>
+    <t>rines</t>
+  </si>
+  <si>
+    <t>ventana</t>
+  </si>
+  <si>
+    <t>puerta</t>
+  </si>
+  <si>
+    <t>asiento</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="3">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:color theme="1"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </x:cellStyleXfs>
-  <x:cellXfs count="3">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:dxfs count="0"/>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-</x:styleSheet>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,73 +417,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F3"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1">
-      <x:c r="A1" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E1" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F1" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2">
-      <x:c r="A2">
-        <x:v>1234456</x:v>
-      </x:c>
-      <x:c r="B2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D2">
-        <x:v>321</x:v>
-      </x:c>
-      <x:c r="E2">
-        <x:v>12.32</x:v>
-      </x:c>
-      <x:c r="F2">
-        <x:v>231</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3">
-      <x:c r="A3">
-        <x:v>2324567</x:v>
-      </x:c>
-      <x:c r="B3" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D3">
-        <x:v>22.3</x:v>
-      </x:c>
-      <x:c r="E3">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="F3">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1234456</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>321</v>
+      </c>
+      <c r="E2">
+        <v>12.32</v>
+      </c>
+      <c r="F2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2324567</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>22.3</v>
+      </c>
+      <c r="E3">
+        <v>22</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4534534</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8576438</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>321</v>
+      </c>
+      <c r="E5">
+        <v>12.32</v>
+      </c>
+      <c r="F5">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6784648</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>22.3</v>
+      </c>
+      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9676555</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>